<commit_message>
monthly update and issue fixes
fix #37
fix #36
fix #23
</commit_message>
<xml_diff>
--- a/control panel.xlsx
+++ b/control panel.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1260" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nnb distribution" sheetId="1" r:id="rId1"/>
@@ -2807,10 +2807,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2957,6 +2957,26 @@
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2032</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2036</v>
       </c>
     </row>
   </sheetData>
@@ -3116,8 +3136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B409"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="O130" sqref="O130"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3832,6 +3852,9 @@
       <c r="A140" s="1">
         <v>43131</v>
       </c>
+      <c r="B140" s="3">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
@@ -3853,162 +3876,166 @@
         <v>43251</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>43280</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>43312</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>43343</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>43371</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>43404</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>43434</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>43465</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>43496</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B152" s="3"/>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>43524</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>43553</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>43585</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>43616</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>43644</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>43677</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>43707</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>43738</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>43769</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>43798</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>43830</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>43861</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B164" s="3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>43889</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>43921</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>43951</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>43980</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44012</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44043</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44074</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44104</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44134</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44165</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44196</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44225</v>
       </c>

</xml_diff>

<commit_message>
26-04-2018 update and new client nnb update
</commit_message>
<xml_diff>
--- a/control panel.xlsx
+++ b/control panel.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E78BDD8-41F2-4FE7-A34E-CA51446C82EE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC46C3BE-FAEF-4DAE-A0DE-5592A14B89D7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1260" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1260" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nnb distribution" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="compound growth" sheetId="3" r:id="rId4"/>
     <sheet name="aua margin" sheetId="4" r:id="rId5"/>
     <sheet name="growth rate" sheetId="5" r:id="rId6"/>
+    <sheet name="nnc pcent total client" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>pms_hlf_aua</t>
   </si>
@@ -122,6 +123,9 @@
   <si>
     <t>cash_service_aua</t>
   </si>
+  <si>
+    <t>nnc pcent total client</t>
+  </si>
 </sst>
 </file>
 
@@ -132,7 +136,7 @@
     <numFmt numFmtId="165" formatCode="0.00000000%"/>
     <numFmt numFmtId="166" formatCode="0.000%"/>
     <numFmt numFmtId="167" formatCode="0.0000000000000000%"/>
-    <numFmt numFmtId="169" formatCode="0.000000000000000%"/>
+    <numFmt numFmtId="168" formatCode="0.000000000000000%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -181,7 +185,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N409"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B126" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7878,4 +7882,1846 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F15434C-F943-4958-9CC1-AD8CDB1EF8AF}">
+  <dimension ref="A1:B409"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>38989</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>39080</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>39171</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>39262</v>
+      </c>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>39353</v>
+      </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>39447</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>39538</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>39629</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>39721</v>
+      </c>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>39813</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>39903</v>
+      </c>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>39994</v>
+      </c>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>40086</v>
+      </c>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>40178</v>
+      </c>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>40268</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>40359</v>
+      </c>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>40451</v>
+      </c>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>40543</v>
+      </c>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>40633</v>
+      </c>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>40724</v>
+      </c>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>40816</v>
+      </c>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>40907</v>
+      </c>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>40998</v>
+      </c>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>41089</v>
+      </c>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>41180</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>41274</v>
+      </c>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>41362</v>
+      </c>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>41453</v>
+      </c>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>41547</v>
+      </c>
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>41639</v>
+      </c>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>41729</v>
+      </c>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>41820</v>
+      </c>
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>41912</v>
+      </c>
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>42004</v>
+      </c>
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>42094</v>
+      </c>
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>42185</v>
+      </c>
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>42277</v>
+      </c>
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>42369</v>
+      </c>
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>42460</v>
+      </c>
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>42551</v>
+      </c>
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>42643</v>
+      </c>
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>42734</v>
+      </c>
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>42825</v>
+      </c>
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>42916</v>
+      </c>
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>43007</v>
+      </c>
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>43098</v>
+      </c>
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>43189</v>
+      </c>
+      <c r="B48" s="2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>43280</v>
+      </c>
+      <c r="B49" s="3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>43371</v>
+      </c>
+      <c r="B50" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>43465</v>
+      </c>
+      <c r="B51" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>43553</v>
+      </c>
+      <c r="B52" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>43644</v>
+      </c>
+      <c r="B53" s="3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>43738</v>
+      </c>
+      <c r="B54" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>43830</v>
+      </c>
+      <c r="B55" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>43921</v>
+      </c>
+      <c r="B56" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>44012</v>
+      </c>
+      <c r="B57" s="3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>44104</v>
+      </c>
+      <c r="B58" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>44196</v>
+      </c>
+      <c r="B59" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>44286</v>
+      </c>
+      <c r="B60" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>44377</v>
+      </c>
+      <c r="B61" s="3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>44469</v>
+      </c>
+      <c r="B62" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>44561</v>
+      </c>
+      <c r="B63" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>44651</v>
+      </c>
+      <c r="B64" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>44742</v>
+      </c>
+      <c r="B65" s="3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>44834</v>
+      </c>
+      <c r="B66" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>44925</v>
+      </c>
+      <c r="B67" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>45016</v>
+      </c>
+      <c r="B68" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B69" s="3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>45198</v>
+      </c>
+      <c r="B70" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>45289</v>
+      </c>
+      <c r="B71" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>45380</v>
+      </c>
+      <c r="B72" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>45471</v>
+      </c>
+      <c r="B73" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>45565</v>
+      </c>
+      <c r="B74" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>45657</v>
+      </c>
+      <c r="B75" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>45747</v>
+      </c>
+      <c r="B76" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>45838</v>
+      </c>
+      <c r="B77" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>45930</v>
+      </c>
+      <c r="B78" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>46022</v>
+      </c>
+      <c r="B79" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>46112</v>
+      </c>
+      <c r="B80" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>46203</v>
+      </c>
+      <c r="B81" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>46295</v>
+      </c>
+      <c r="B82" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B83" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>46477</v>
+      </c>
+      <c r="B84" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>46568</v>
+      </c>
+      <c r="B85" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>46660</v>
+      </c>
+      <c r="B86" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>46752</v>
+      </c>
+      <c r="B87" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>46843</v>
+      </c>
+      <c r="B88" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>46934</v>
+      </c>
+      <c r="B89" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>47025</v>
+      </c>
+      <c r="B90" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>47116</v>
+      </c>
+      <c r="B91" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>47207</v>
+      </c>
+      <c r="B92" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>47298</v>
+      </c>
+      <c r="B93" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>47389</v>
+      </c>
+      <c r="B94" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>47483</v>
+      </c>
+      <c r="B95" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>47571</v>
+      </c>
+      <c r="B96" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>47662</v>
+      </c>
+      <c r="B97" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>47756</v>
+      </c>
+      <c r="B98" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>47848</v>
+      </c>
+      <c r="B99" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>47938</v>
+      </c>
+      <c r="B100" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>48029</v>
+      </c>
+      <c r="B101" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>48121</v>
+      </c>
+      <c r="B102" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>48213</v>
+      </c>
+      <c r="B103" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>48304</v>
+      </c>
+      <c r="B104" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>48395</v>
+      </c>
+      <c r="B105" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>48487</v>
+      </c>
+      <c r="B106" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>48579</v>
+      </c>
+      <c r="B107" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>48669</v>
+      </c>
+      <c r="B108" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>48760</v>
+      </c>
+      <c r="B109" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>48852</v>
+      </c>
+      <c r="B110" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>48943</v>
+      </c>
+      <c r="B111" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>49034</v>
+      </c>
+      <c r="B112" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>49125</v>
+      </c>
+      <c r="B113" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>49216</v>
+      </c>
+      <c r="B114" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>49307</v>
+      </c>
+      <c r="B115" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>49398</v>
+      </c>
+      <c r="B116" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>49489</v>
+      </c>
+      <c r="B117" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>49580</v>
+      </c>
+      <c r="B118" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>49674</v>
+      </c>
+      <c r="B119" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>49765</v>
+      </c>
+      <c r="B120" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>49856</v>
+      </c>
+      <c r="B121" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>49948</v>
+      </c>
+      <c r="B122" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>50040</v>
+      </c>
+      <c r="B123" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>50130</v>
+      </c>
+      <c r="B124" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>50221</v>
+      </c>
+      <c r="B125" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>50313</v>
+      </c>
+      <c r="B126" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>50405</v>
+      </c>
+      <c r="B127" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>50495</v>
+      </c>
+      <c r="B128" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>50586</v>
+      </c>
+      <c r="B129" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>50678</v>
+      </c>
+      <c r="B130" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>50770</v>
+      </c>
+      <c r="B131" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>50860</v>
+      </c>
+      <c r="B132" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>50951</v>
+      </c>
+      <c r="B133" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>51043</v>
+      </c>
+      <c r="B134" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>51134</v>
+      </c>
+      <c r="B135" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>51225</v>
+      </c>
+      <c r="B136" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>51316</v>
+      </c>
+      <c r="B137" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="1"/>
+      <c r="B141" s="1"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="1"/>
+      <c r="B142" s="1"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="1"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="1"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="1"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="1"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="1"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="1"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="1"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="1"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="1"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="1"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="1"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="1"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="1"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="1"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="1"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="1"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="1"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="1"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="1"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="1"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="1"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="1"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="1"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="1"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="1"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="1"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="1"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="1"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="1"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="1"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="1"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="1"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="1"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="1"/>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="1"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="1"/>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="1"/>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="1"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="1"/>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="1"/>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="1"/>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="1"/>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="1"/>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="1"/>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="1"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="1"/>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="1"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="1"/>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="1"/>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="1"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="1"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="1"/>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="1"/>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="1"/>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="1"/>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="1"/>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="1"/>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="1"/>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="1"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="1"/>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="1"/>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="1"/>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="1"/>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="1"/>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="1"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="1"/>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="1"/>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="1"/>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="1"/>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="1"/>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="1"/>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="1"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="1"/>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="1"/>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="1"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="1"/>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="1"/>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="1"/>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="1"/>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="1"/>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="1"/>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="1"/>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="1"/>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="1"/>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="1"/>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="1"/>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="1"/>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="1"/>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="1"/>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="1"/>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="1"/>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="1"/>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="1"/>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="1"/>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="1"/>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="1"/>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="1"/>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="1"/>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="1"/>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="1"/>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="1"/>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="1"/>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="1"/>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="1"/>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="1"/>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="1"/>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="1"/>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="1"/>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="1"/>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="1"/>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="1"/>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="1"/>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="1"/>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="1"/>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="1"/>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="1"/>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="1"/>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="1"/>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="1"/>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="1"/>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="1"/>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="1"/>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="1"/>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="1"/>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="1"/>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" s="1"/>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="1"/>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="1"/>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="1"/>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="1"/>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="1"/>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="1"/>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="1"/>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" s="1"/>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="1"/>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="1"/>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="1"/>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="1"/>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="1"/>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="1"/>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="1"/>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" s="1"/>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" s="1"/>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="1"/>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" s="1"/>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" s="1"/>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" s="1"/>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" s="1"/>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" s="1"/>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" s="1"/>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" s="1"/>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" s="1"/>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" s="1"/>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" s="1"/>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" s="1"/>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="1"/>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" s="1"/>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" s="1"/>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" s="1"/>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" s="1"/>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" s="1"/>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" s="1"/>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" s="1"/>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" s="1"/>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" s="1"/>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" s="1"/>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" s="1"/>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" s="1"/>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" s="1"/>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" s="1"/>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" s="1"/>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" s="1"/>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" s="1"/>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" s="1"/>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" s="1"/>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" s="1"/>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" s="1"/>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" s="1"/>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" s="1"/>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" s="1"/>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" s="1"/>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" s="1"/>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" s="1"/>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" s="1"/>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" s="1"/>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" s="1"/>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" s="1"/>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" s="1"/>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" s="1"/>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" s="1"/>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" s="1"/>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" s="1"/>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" s="1"/>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" s="1"/>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" s="1"/>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" s="1"/>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" s="1"/>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" s="1"/>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" s="1"/>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" s="1"/>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" s="1"/>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" s="1"/>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" s="1"/>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" s="1"/>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" s="1"/>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" s="1"/>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" s="1"/>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" s="1"/>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" s="1"/>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" s="1"/>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" s="1"/>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" s="1"/>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" s="1"/>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" s="1"/>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" s="1"/>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" s="1"/>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" s="1"/>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" s="1"/>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" s="1"/>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" s="1"/>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" s="1"/>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" s="1"/>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" s="1"/>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" s="1"/>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" s="1"/>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" s="1"/>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" s="1"/>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" s="1"/>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" s="1"/>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" s="1"/>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" s="1"/>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" s="1"/>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" s="1"/>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" s="1"/>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" s="1"/>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" s="1"/>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" s="1"/>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" s="1"/>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" s="1"/>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" s="1"/>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" s="1"/>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" s="1"/>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" s="1"/>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" s="1"/>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" s="1"/>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" s="1"/>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" s="1"/>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" s="1"/>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" s="1"/>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" s="1"/>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" s="1"/>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" s="1"/>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
10-05-2018 update interest rate and compound rate adjustment
</commit_message>
<xml_diff>
--- a/control panel.xlsx
+++ b/control panel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC97433D-AE53-468F-957E-3951ADED39FA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16023AC7-F69E-4CD3-9C2D-1E7D8E58C996}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1260" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1260" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nnb distribution" sheetId="1" r:id="rId1"/>
@@ -3279,8 +3279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B409"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="E151" sqref="E151"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="N147" sqref="N147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4046,6 +4046,9 @@
       <c r="A149" s="1">
         <v>43404</v>
       </c>
+      <c r="B149" s="3">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
@@ -4061,9 +4064,7 @@
       <c r="A152" s="1">
         <v>43496</v>
       </c>
-      <c r="B152" s="3">
-        <v>0.06</v>
-      </c>
+      <c r="B152" s="3"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
@@ -7888,7 +7889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F15434C-F943-4958-9CC1-AD8CDB1EF8AF}">
   <dimension ref="A1:B409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="O60" sqref="O60"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
funds data updated 27-07-2018
</commit_message>
<xml_diff>
--- a/control panel.xlsx
+++ b/control panel.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6E6845-6BCB-425C-B905-002EE40DDF12}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617A4CF4-7AB3-430C-916E-B82EF9E9F890}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1680" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2100" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nnb distribution" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,11 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -3137,8 +3142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16FFE29E-9431-479B-A1F7-074B6658152B}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3198,7 +3203,7 @@
         <v>2017</v>
       </c>
       <c r="B11">
-        <v>0.19</v>
+        <v>0.1925</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -7471,7 +7476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A942FEE-B827-46F7-9078-F9FB4C734CE0}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
11th Oct update and added fx_effects on funds
</commit_message>
<xml_diff>
--- a/control panel.xlsx
+++ b/control panel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD1EB23-A053-4376-8307-37920245E5B1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD40238-5DE7-4BBA-8741-BC994DDAA8F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5880" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nnb distribution" sheetId="1" r:id="rId1"/>
@@ -8358,8 +8358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F15434C-F943-4958-9CC1-AD8CDB1EF8AF}">
   <dimension ref="A1:B409"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8624,7 +8624,7 @@
         <v>43371</v>
       </c>
       <c r="B50" s="10">
-        <v>2.3E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -10148,7 +10148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB3FCC0-CE90-4C6B-A07F-3125A3989D1D}">
   <dimension ref="A1:C409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+    <sheetView topLeftCell="A146" workbookViewId="0">
       <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
03-01-2019 update of cash margin assumptions
</commit_message>
<xml_diff>
--- a/control panel.xlsx
+++ b/control panel.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{759912B8-E9F5-4C0D-9E37-06D5DDBD1CFA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7346A51F-EA79-4C95-BF17-F3EEC99EE6E2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nnb distribution" sheetId="1" r:id="rId1"/>
@@ -7616,8 +7616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A942FEE-B827-46F7-9078-F9FB4C734CE0}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7860,7 +7860,7 @@
         <v>0.06</v>
       </c>
       <c r="I6" s="2">
-        <v>2.47E-2</v>
+        <v>-1.2E-2</v>
       </c>
       <c r="K6" s="2">
         <v>-0.5</v>
@@ -8356,8 +8356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F15434C-F943-4958-9CC1-AD8CDB1EF8AF}">
   <dimension ref="A1:B409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10146,8 +10146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB3FCC0-CE90-4C6B-A07F-3125A3989D1D}">
   <dimension ref="A1:C409"/>
   <sheetViews>
-    <sheetView topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="C159" sqref="C159"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="H137" sqref="H137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10720,82 +10720,88 @@
         <v>42277</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>42307</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>42338</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>42369</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>42398</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B116" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="C116" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>42429</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>42460</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>42489</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>42521</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>42551</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>42580</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>42613</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>42643</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>42674</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>42704</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>42734</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>42766</v>
       </c>

</xml_diff>

<commit_message>
16-01-2019 update and included corporate bonds return in other funds calculation
</commit_message>
<xml_diff>
--- a/control panel.xlsx
+++ b/control panel.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{24CB967B-1649-47BD-AB70-C8965D90A759}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1598C6B5-4C28-4DA1-9DB4-46163743D114}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nnb distribution" sheetId="1" r:id="rId1"/>
@@ -478,11 +478,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N409"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B143" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B140" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G155" sqref="G155"/>
+      <selection pane="bottomRight" activeCell="L148" sqref="L148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3106,8 +3106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8439,8 +8439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F15434C-F943-4958-9CC1-AD8CDB1EF8AF}">
   <dimension ref="A1:B409"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8729,7 +8729,7 @@
         <v>43644</v>
       </c>
       <c r="B53" s="10">
-        <v>3.2000000000000001E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -10229,7 +10229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB3FCC0-CE90-4C6B-A07F-3125A3989D1D}">
   <dimension ref="A1:C409"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
+    <sheetView topLeftCell="A106" workbookViewId="0">
       <selection activeCell="J127" sqref="J127"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changed year on general
</commit_message>
<xml_diff>
--- a/control panel.xlsx
+++ b/control panel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1598C6B5-4C28-4DA1-9DB4-46163743D114}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83C5468-9361-4C8E-B56A-79609DAB6AB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nnb distribution" sheetId="1" r:id="rId1"/>
@@ -478,7 +478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N409"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B140" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3106,8 +3106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3184,7 +3184,7 @@
         <v>2019</v>
       </c>
       <c r="B13" s="3">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed a bug on calculating compounded rate for future aua
</commit_message>
<xml_diff>
--- a/control panel.xlsx
+++ b/control panel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33167841-99FE-4A3B-866B-9B2A978C482A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C06451-82CE-4F36-858E-1A204C008268}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3501,8 +3501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4323,6 +4323,7 @@
       <c r="A158" s="1">
         <v>43677</v>
       </c>
+      <c r="B158" s="3"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="1">

</xml_diff>

<commit_message>
amended no of shares used to calculate EPS and fixed control panel index problem
</commit_message>
<xml_diff>
--- a/control panel.xlsx
+++ b/control panel.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83C5468-9361-4C8E-B56A-79609DAB6AB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833EB89A-3765-4302-BA9A-A4A33890AF30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nnb distribution" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="nnc pcent total client" sheetId="7" r:id="rId7"/>
     <sheet name="cash interest rebate" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -479,7 +479,7 @@
   <dimension ref="A1:N409"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B341" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="L148" sqref="L148"/>
@@ -3106,8 +3106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3283,10 +3283,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16FFE29E-9431-479B-A1F7-074B6658152B}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3445,6 +3445,26 @@
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2036</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2040</v>
       </c>
     </row>
   </sheetData>
@@ -3456,8 +3476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B409"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="B157" sqref="B157"/>
+    <sheetView topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="L153" sqref="L153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4247,10 +4267,16 @@
       <c r="A153" s="1">
         <v>43524</v>
       </c>
+      <c r="B153" s="3">
+        <v>0.36</v>
+      </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>43553</v>
+      </c>
+      <c r="B154" s="3">
+        <v>0.06</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -5539,10 +5565,10 @@
   <dimension ref="A1:E409"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C139" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B340" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E147" sqref="E147"/>
+      <selection pane="bottomRight" activeCell="A355" sqref="A355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7697,10 +7723,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A942FEE-B827-46F7-9078-F9FB4C734CE0}">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8430,6 +8456,21 @@
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
     </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>49307</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>49489</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>49674</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8439,7 +8480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F15434C-F943-4958-9CC1-AD8CDB1EF8AF}">
   <dimension ref="A1:B409"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A131" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -10229,7 +10270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB3FCC0-CE90-4C6B-A07F-3125A3989D1D}">
   <dimension ref="A1:C409"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
+    <sheetView topLeftCell="A373" workbookViewId="0">
       <selection activeCell="J127" sqref="J127"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added some extra functionality and adjusted FSCS assumption
</commit_message>
<xml_diff>
--- a/control panel.xlsx
+++ b/control panel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833EB89A-3765-4302-BA9A-A4A33890AF30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A4F146-E907-4D28-8670-CCEE4ECA11B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7725,8 +7725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A942FEE-B827-46F7-9078-F9FB4C734CE0}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8001,7 +8001,7 @@
         <v>0.05</v>
       </c>
       <c r="K7" s="3">
-        <v>0.3</v>
+        <v>15.6</v>
       </c>
       <c r="L7" s="2">
         <v>0.05</v>
@@ -8024,7 +8024,7 @@
         <v>43830</v>
       </c>
       <c r="K8" s="2">
-        <v>-0.12</v>
+        <v>-0.5</v>
       </c>
       <c r="L8" s="3">
         <v>0.03</v>
@@ -8480,7 +8480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F15434C-F943-4958-9CC1-AD8CDB1EF8AF}">
   <dimension ref="A1:B409"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
+    <sheetView topLeftCell="A86" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adjusted cash rebates parameters
</commit_message>
<xml_diff>
--- a/control panel.xlsx
+++ b/control panel.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A4F146-E907-4D28-8670-CCEE4ECA11B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC8E918-0D61-401C-A21B-0837BD4A7E87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" tabRatio="848" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nnb distribution" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,15 @@
     <sheet name="nnc pcent total client" sheetId="7" r:id="rId7"/>
     <sheet name="cash interest rebate" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -7725,7 +7730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A942FEE-B827-46F7-9078-F9FB4C734CE0}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -8480,8 +8485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F15434C-F943-4958-9CC1-AD8CDB1EF8AF}">
   <dimension ref="A1:B409"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8762,7 +8767,7 @@
         <v>43553</v>
       </c>
       <c r="B52" s="10">
-        <v>0.04</v>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -8770,7 +8775,7 @@
         <v>43644</v>
       </c>
       <c r="B53" s="10">
-        <v>4.2000000000000003E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -10270,8 +10275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB3FCC0-CE90-4C6B-A07F-3125A3989D1D}">
   <dimension ref="A1:C409"/>
   <sheetViews>
-    <sheetView topLeftCell="A373" workbookViewId="0">
-      <selection activeCell="J127" sqref="J127"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="P150" sqref="P150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11085,12 +11090,6 @@
       <c r="A158" s="1">
         <v>43677</v>
       </c>
-      <c r="B158" s="2">
-        <v>3.5000000000000001E-3</v>
-      </c>
-      <c r="C158" s="2">
-        <v>3.0000000000000001E-3</v>
-      </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
@@ -11102,82 +11101,88 @@
         <v>43738</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>43769</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>43798</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>43830</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>43861</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>43889</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>43921</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>43951</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B167" s="2">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="C167" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>43980</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44012</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44043</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44074</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44104</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44134</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44165</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44196</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44225</v>
       </c>

</xml_diff>